<commit_message>
backlog update and commenting apis v1.2
</commit_message>
<xml_diff>
--- a/Documents/Team Backlog.xlsx
+++ b/Documents/Team Backlog.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sharb\OneDrive\Documents\GitHub\Sprints_AirConditioningSystem\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sprints_SimpleATM\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97431D87-7E27-4C67-A3F2-93AC9B1B39BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{875C6DCD-AFAF-4A5F-9F21-083CA0FCED6F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="70">
   <si>
     <t>Task Name</t>
   </si>
@@ -57,24 +56,15 @@
     <t>3 hours</t>
   </si>
   <si>
-    <t>4 hours</t>
-  </si>
-  <si>
     <t>2 hours</t>
   </si>
   <si>
-    <t>1.5 hour</t>
-  </si>
-  <si>
     <t>30 minutes</t>
   </si>
   <si>
     <t>45 minutes</t>
   </si>
   <si>
-    <t>Sherif Ashraf</t>
-  </si>
-  <si>
     <t>20 minutes</t>
   </si>
   <si>
@@ -84,100 +74,172 @@
     <t>Alaa Hisham</t>
   </si>
   <si>
-    <t>Integrate all Drivers</t>
-  </si>
-  <si>
-    <t>Documentation</t>
-  </si>
-  <si>
-    <t>MCAL_DIO_DESIGN</t>
-  </si>
-  <si>
-    <t>MCAL_DIO_IMPLEMENTATION</t>
-  </si>
-  <si>
-    <t>MCAL_DIO_TESTING</t>
-  </si>
-  <si>
-    <t>ECU_LCD_DESIGN</t>
-  </si>
-  <si>
-    <t>ECU_LCD_IMPLEMENTATION</t>
-  </si>
-  <si>
-    <t>ECU_LCD_TESTING</t>
-  </si>
-  <si>
-    <t>ECU_KEYPAD_DESIGN</t>
-  </si>
-  <si>
-    <t>ECU_KEYPAD_IMPLEMENTATION</t>
-  </si>
-  <si>
-    <t>ECU_KEYPAD_TESTING</t>
-  </si>
-  <si>
-    <t>MCAL_ADC_DESIGN</t>
-  </si>
-  <si>
-    <t>MCAL_ADC_IMPLEMENTATION</t>
-  </si>
-  <si>
-    <t>MCAL_ADC_TESTING</t>
-  </si>
-  <si>
-    <t>ECU_BUZZER_DESIGN</t>
-  </si>
-  <si>
-    <t>ECU_BUZZER_IMPLEMENTATION</t>
-  </si>
-  <si>
-    <t>ECU_BUZZER_TESTING</t>
-  </si>
-  <si>
-    <t>ECU_TEMPSENSOR_DESIGN</t>
-  </si>
-  <si>
-    <t>ECU_TEMPSENSOR_IMPLEMENTATION</t>
-  </si>
-  <si>
-    <t>ECU_TEMPSENSOR_TESTING</t>
-  </si>
-  <si>
-    <t>APP_DESIGN</t>
-  </si>
-  <si>
-    <t>APP_IMPLEMENTATION</t>
-  </si>
-  <si>
-    <t>APP_TESTING</t>
-  </si>
-  <si>
-    <t>team</t>
-  </si>
-  <si>
-    <t>10 hours</t>
-  </si>
-  <si>
-    <t>110 minutes</t>
-  </si>
-  <si>
-    <t>TIMER_DESIGN</t>
-  </si>
-  <si>
-    <t>TIMER_IMPLEMENTATION</t>
-  </si>
-  <si>
-    <t>TIMER_TESTING</t>
-  </si>
-  <si>
     <t>5 minutes</t>
+  </si>
+  <si>
+    <t>MCAL_I2C_DESIGN</t>
+  </si>
+  <si>
+    <t>MCAL_I2C_TEST</t>
+  </si>
+  <si>
+    <t>MCAL_I2C_IMPLEMENTATION</t>
+  </si>
+  <si>
+    <t>MCAL_TIMER2_DESIGN</t>
+  </si>
+  <si>
+    <t>MCAL_TIMER2_IMPLEMENTATION</t>
+  </si>
+  <si>
+    <t>MCAL_TIMER2_TESTING</t>
+  </si>
+  <si>
+    <t>ECUAL_HTIMER2</t>
+  </si>
+  <si>
+    <t>CARD_terminalPinGet API</t>
+  </si>
+  <si>
+    <t>MCAL_USART_DESIGN</t>
+  </si>
+  <si>
+    <t>MCAL_USART_IMPLEMENTATION</t>
+  </si>
+  <si>
+    <t>MCAL_USART_TESTING</t>
+  </si>
+  <si>
+    <t>ECUAL_HEXTINT</t>
+  </si>
+  <si>
+    <t>ECUAL_HUSART</t>
+  </si>
+  <si>
+    <t>Card_terminalPanGet API</t>
+  </si>
+  <si>
+    <t>ATM_Get_pin API</t>
+  </si>
+  <si>
+    <t>ATM_get_amount_left API</t>
+  </si>
+  <si>
+    <t>10 minutes</t>
+  </si>
+  <si>
+    <t>ATM_ENTER/ZERO_Button API</t>
+  </si>
+  <si>
+    <t>90 minutes</t>
+  </si>
+  <si>
+    <t>MCAL_SPI_DESIGN</t>
+  </si>
+  <si>
+    <t>MCAL_SPI_IMPLEMENTATION</t>
+  </si>
+  <si>
+    <t>MCAL_SPI_TESTING</t>
+  </si>
+  <si>
+    <t>MCAL_TIMER0 Module</t>
+  </si>
+  <si>
+    <t>MCAL_DIO Module</t>
+  </si>
+  <si>
+    <t>ECUAL_BUTTON Module</t>
+  </si>
+  <si>
+    <t>ECUAL_LCD Module</t>
+  </si>
+  <si>
+    <t>MCAL_EXTINT Module</t>
+  </si>
+  <si>
+    <t>ECUAL_KEYPAD Module</t>
+  </si>
+  <si>
+    <t>ECUAL_BUZZER Module</t>
+  </si>
+  <si>
+    <t>CARD_MatchPINs API</t>
+  </si>
+  <si>
+    <t>ATM_GetCardData API</t>
+  </si>
+  <si>
+    <t>ATM_ApprovedCard API</t>
+  </si>
+  <si>
+    <t>ECUAL_HSPI_DESIGN</t>
+  </si>
+  <si>
+    <t>ECUAL_HSPI_IMPLEMENTATION</t>
+  </si>
+  <si>
+    <t>ECUAL_HSPI_TESTING</t>
+  </si>
+  <si>
+    <t>ECUAL_EEPROM_DESIGN</t>
+  </si>
+  <si>
+    <t>ECUAL_EEPROM_IMPLEMENTATION</t>
+  </si>
+  <si>
+    <t>ECUAL_EEPROM_TESTING</t>
+  </si>
+  <si>
+    <t>ATM_PIN_checkPinMatching API</t>
+  </si>
+  <si>
+    <t>ATM_deinitAtm API</t>
+  </si>
+  <si>
+    <t>CARD_SaveCardData API</t>
+  </si>
+  <si>
+    <t>CARD_READCardData API</t>
+  </si>
+  <si>
+    <t>Sherif Khedr</t>
+  </si>
+  <si>
+    <t>6 hours</t>
+  </si>
+  <si>
+    <t>8 hours</t>
+  </si>
+  <si>
+    <t>ATM_DATABASE_CHECKING Module</t>
+  </si>
+  <si>
+    <t>Sprinters</t>
+  </si>
+  <si>
+    <t>INTEGRATION</t>
+  </si>
+  <si>
+    <t>3 hour</t>
+  </si>
+  <si>
+    <t>SIMULATION_DEBUGGING</t>
+  </si>
+  <si>
+    <t>HARDWARE_DEBUGGING</t>
+  </si>
+  <si>
+    <t>4 days and counting</t>
+  </si>
+  <si>
+    <t>2 days</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -575,11 +637,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C123E326-AE56-4BD1-BFE1-3D77BAFFAE7E}">
-  <dimension ref="A1:F27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E48" sqref="C48:E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +677,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -624,7 +686,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>8</v>
@@ -635,7 +697,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -644,10 +706,10 @@
         <v>100</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -655,7 +717,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
@@ -664,10 +726,10 @@
         <v>100</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -675,7 +737,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
@@ -684,10 +746,10 @@
         <v>100</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -695,7 +757,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
@@ -704,10 +766,10 @@
         <v>100</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -715,7 +777,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
@@ -724,10 +786,10 @@
         <v>100</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -735,19 +797,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1">
         <v>100</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -755,19 +817,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" s="1">
         <v>100</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -775,19 +837,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1">
         <v>100</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -795,19 +857,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D11" s="1">
         <v>100</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -815,10 +877,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1">
         <v>100</v>
@@ -827,7 +889,7 @@
         <v>11</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -835,19 +897,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D13" s="1">
         <v>100</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -855,19 +917,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1">
         <v>100</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -875,19 +937,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D15" s="1">
         <v>100</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -895,19 +957,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D16" s="1">
         <v>100</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -915,19 +977,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1">
+        <v>100</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="1">
-        <v>100</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="F17" s="5" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -935,19 +997,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D18" s="1">
         <v>100</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -955,19 +1017,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D19" s="1">
         <v>100</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -975,19 +1037,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D20" s="1">
         <v>100</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -995,19 +1057,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D21" s="1">
         <v>100</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1015,19 +1077,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D22" s="1">
         <v>100</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1035,19 +1097,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D23" s="1">
         <v>100</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1055,19 +1117,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D24" s="1">
         <v>100</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1075,19 +1137,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="D25" s="1">
         <v>100</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1095,10 +1157,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="D26" s="1">
         <v>100</v>
@@ -1107,7 +1169,7 @@
         <v>11</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1115,19 +1177,379 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="1">
+        <v>100</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="1">
+        <v>100</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="1">
+        <v>100</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="1">
+        <v>100</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="1">
+        <v>100</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="1">
+        <v>100</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="1">
+        <v>100</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="1">
+        <v>100</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="1">
+        <v>100</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="1">
+        <v>100</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="1">
+        <v>100</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38" s="1">
+        <v>100</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="1">
+        <v>100</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" s="1">
+        <v>100</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="1">
+        <v>100</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="1">
+        <v>100</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>42</v>
       </c>
-      <c r="D27" s="1">
-        <v>100</v>
-      </c>
-      <c r="E27" s="5" t="s">
+      <c r="B43" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" s="1">
+        <v>100</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F27" s="5" t="s">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" s="1">
+        <v>100</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
         <v>44</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" s="1">
+        <v>85</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>